<commit_message>
update de portas com botoes agora
</commit_message>
<xml_diff>
--- a/Docs/PINAGEM.xlsx
+++ b/Docs/PINAGEM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flavi\Documents\GitHub\ChoppBot\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconr\Documents\GitHub\choppbot\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>SD</t>
   </si>
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -584,28 +584,28 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>9</v>
@@ -630,7 +630,7 @@
       <c r="W3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AB3" s="7" t="s">
         <v>12</v>
@@ -704,7 +704,7 @@
       <c r="W5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AB5" s="6" t="s">
         <v>10</v>
@@ -737,12 +737,6 @@
       </c>
       <c r="W6" s="1"/>
       <c r="Z6" s="1"/>
-      <c r="AA6">
-        <v>44</v>
-      </c>
-      <c r="AB6" s="10" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>

</xml_diff>

<commit_message>
finalizacao do prototipo e pinos
prototipo terminado e tds os pinos debugados
</commit_message>
<xml_diff>
--- a/Docs/PINAGEM.xlsx
+++ b/Docs/PINAGEM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconr\Documents\GitHub\choppbot\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD785EA-83D8-4F13-A8B4-78DBBE397721}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3E4AD4-68A5-4370-95DA-0D67793DB52A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
   <si>
     <t>SD</t>
   </si>
@@ -157,7 +157,13 @@
     <t>interf tela</t>
   </si>
   <si>
-    <t>inter sd</t>
+    <t>am + rx</t>
+  </si>
+  <si>
+    <t>JP 5</t>
+  </si>
+  <si>
+    <t>lado botao</t>
   </si>
 </sst>
 </file>
@@ -206,7 +212,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +290,16 @@
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
+    </fill>
+    <fill>
+      <gradientFill>
+        <stop position="0">
+          <color rgb="FFFFFF00"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF7030A0"/>
+        </stop>
+      </gradientFill>
     </fill>
   </fills>
   <borders count="5">
@@ -416,9 +432,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,12 +440,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -450,17 +457,26 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -780,7 +796,7 @@
   <dimension ref="A1:AM999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -800,82 +816,83 @@
     <col min="25" max="25" width="3" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.85546875" style="28" customWidth="1"/>
-    <col min="29" max="30" width="8.7109375" style="28" customWidth="1"/>
-    <col min="31" max="31" width="3.85546875" style="28" customWidth="1"/>
+    <col min="28" max="28" width="3.85546875" style="27" customWidth="1"/>
+    <col min="29" max="29" width="5.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.7109375" style="27" customWidth="1"/>
+    <col min="31" max="31" width="3.85546875" style="27" customWidth="1"/>
     <col min="32" max="32" width="3" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="3.85546875" customWidth="1"/>
     <col min="36" max="37" width="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.85546875" customWidth="1"/>
     <col min="39" max="39" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="25" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="25" t="s">
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="25" t="s">
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="25" t="s">
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="25" t="s">
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="25" t="s">
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="30" t="s">
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="25" t="s">
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="26"/>
-      <c r="AJ1" s="25" t="s">
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="26"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="25"/>
     </row>
     <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40">
-        <v>53</v>
+      <c r="A2" s="41">
+        <v>11</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>12</v>
@@ -924,17 +941,17 @@
         <v>25</v>
       </c>
       <c r="T2" s="11"/>
-      <c r="U2" s="36">
-        <v>21</v>
+      <c r="U2" s="7">
+        <v>12</v>
       </c>
-      <c r="V2" s="22" t="s">
-        <v>18</v>
+      <c r="V2" s="2" t="s">
+        <v>17</v>
       </c>
-      <c r="W2" s="20" t="s">
-        <v>20</v>
+      <c r="W2" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="X2" s="11"/>
-      <c r="Y2" s="36">
+      <c r="Y2" s="33">
         <v>9</v>
       </c>
       <c r="Z2" s="22" t="s">
@@ -944,10 +961,10 @@
         <v>25</v>
       </c>
       <c r="AB2" s="11"/>
-      <c r="AC2" s="31" t="s">
+      <c r="AC2" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="AD2" s="31"/>
+      <c r="AD2" s="36"/>
       <c r="AE2" s="11"/>
       <c r="AF2" s="22">
         <v>45</v>
@@ -965,13 +982,13 @@
       <c r="AK2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="AL2" s="12" t="s">
-        <v>25</v>
+      <c r="AL2" s="40" t="s">
+        <v>45</v>
       </c>
       <c r="AM2" s="11"/>
     </row>
     <row r="3" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41">
+      <c r="A3" s="8">
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -985,14 +1002,14 @@
       <c r="L3" s="11"/>
       <c r="P3" s="11"/>
       <c r="T3" s="11"/>
-      <c r="U3" s="37">
-        <v>22</v>
+      <c r="U3" s="21">
+        <v>13</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>17</v>
+      <c r="V3" s="22" t="s">
+        <v>18</v>
       </c>
-      <c r="W3" s="13" t="s">
-        <v>26</v>
+      <c r="W3" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="X3" s="11"/>
       <c r="Y3" s="2">
@@ -1005,11 +1022,11 @@
         <v>21</v>
       </c>
       <c r="AB3" s="11"/>
-      <c r="AC3" s="38">
-        <v>21</v>
+      <c r="AC3" s="39">
+        <v>20</v>
       </c>
-      <c r="AD3" s="16" t="s">
-        <v>27</v>
+      <c r="AD3" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="AE3" s="11"/>
       <c r="AF3" s="2">
@@ -1034,7 +1051,7 @@
       <c r="AM3" s="11"/>
     </row>
     <row r="4" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37">
+      <c r="A4" s="7">
         <v>50</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1059,11 +1076,11 @@
         <v>23</v>
       </c>
       <c r="AB4" s="11"/>
-      <c r="AC4" s="38">
-        <v>20</v>
+      <c r="AC4" s="39">
+        <v>21</v>
       </c>
-      <c r="AD4" s="17" t="s">
-        <v>18</v>
+      <c r="AD4" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="AE4" s="11"/>
       <c r="AF4" s="2">
@@ -1088,7 +1105,7 @@
       <c r="AM4" s="11"/>
     </row>
     <row r="5" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37">
+      <c r="A5" s="7">
         <v>52</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1113,8 +1130,6 @@
         <v>27</v>
       </c>
       <c r="AB5" s="11"/>
-      <c r="AC5" s="22"/>
-      <c r="AD5" s="22"/>
       <c r="AE5" s="11"/>
       <c r="AI5" s="11"/>
       <c r="AM5" s="11"/>
@@ -1127,9 +1142,7 @@
       <c r="L6" s="11"/>
       <c r="P6" s="11"/>
       <c r="T6" s="11"/>
-      <c r="V6" s="15" t="s">
-        <v>24</v>
-      </c>
+      <c r="V6" s="15"/>
       <c r="X6" s="11"/>
       <c r="Y6" s="2">
         <v>53</v>
@@ -1141,26 +1154,22 @@
         <v>18</v>
       </c>
       <c r="AB6" s="11"/>
-      <c r="AC6" s="31" t="s">
+      <c r="AC6" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="AD6" s="31"/>
+      <c r="AD6" s="36"/>
       <c r="AE6" s="11"/>
       <c r="AI6" s="11"/>
       <c r="AM6" s="11"/>
     </row>
     <row r="7" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
-        <v>24</v>
-      </c>
+      <c r="B7" s="15"/>
       <c r="D7" s="11"/>
       <c r="H7" s="11"/>
       <c r="L7" s="11"/>
       <c r="P7" s="11"/>
       <c r="T7" s="11"/>
-      <c r="V7" s="15" t="s">
-        <v>44</v>
-      </c>
+      <c r="V7" s="15"/>
       <c r="X7" s="11"/>
       <c r="AB7" s="11"/>
       <c r="AC7" s="19" t="s">
@@ -1174,9 +1183,7 @@
       <c r="AM7" s="11"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
-        <v>45</v>
-      </c>
+      <c r="B8" s="34"/>
       <c r="D8" s="1"/>
       <c r="H8" s="11"/>
       <c r="L8" s="11"/>
@@ -1208,7 +1215,7 @@
       <c r="AC9" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="AD9" s="32" t="s">
+      <c r="AD9" s="29" t="s">
         <v>36</v>
       </c>
       <c r="AE9" s="1"/>
@@ -1249,7 +1256,7 @@
       <c r="AC11" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="AD11" s="33" t="s">
+      <c r="AD11" s="30" t="s">
         <v>39</v>
       </c>
       <c r="AE11" s="1"/>
@@ -1267,7 +1274,7 @@
       <c r="AC12" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="AD12" s="34" t="s">
+      <c r="AD12" s="31" t="s">
         <v>22</v>
       </c>
       <c r="AE12" s="1"/>
@@ -1294,10 +1301,10 @@
       <c r="T14" s="1"/>
       <c r="X14" s="1"/>
       <c r="AB14" s="1"/>
-      <c r="AC14" s="31" t="s">
+      <c r="AC14" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="AD14" s="31"/>
+      <c r="AD14" s="36"/>
       <c r="AE14" s="1"/>
       <c r="AI14" s="1"/>
       <c r="AM14" s="1"/>
@@ -1331,7 +1338,7 @@
       <c r="AC16" s="19">
         <v>4</v>
       </c>
-      <c r="AD16" s="35" t="s">
+      <c r="AD16" s="32" t="s">
         <v>21</v>
       </c>
       <c r="AE16" s="1"/>
@@ -1385,7 +1392,7 @@
       <c r="AC19" s="19">
         <v>7</v>
       </c>
-      <c r="AD19" s="33" t="s">
+      <c r="AD19" s="30" t="s">
         <v>39</v>
       </c>
       <c r="AE19" s="1"/>
@@ -1414,10 +1421,10 @@
       <c r="T21" s="1"/>
       <c r="X21" s="1"/>
       <c r="AB21" s="1"/>
-      <c r="AC21" s="31" t="s">
+      <c r="AC21" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="AD21" s="31"/>
+      <c r="AD21" s="36"/>
       <c r="AE21" s="1"/>
       <c r="AI21" s="1"/>
       <c r="AM21" s="1"/>
@@ -1448,10 +1455,10 @@
       <c r="T23" s="1"/>
       <c r="X23" s="1"/>
       <c r="AB23" s="1"/>
-      <c r="AC23" s="38">
+      <c r="AC23" s="19">
         <v>9</v>
       </c>
-      <c r="AD23" s="35" t="s">
+      <c r="AD23" s="32" t="s">
         <v>21</v>
       </c>
       <c r="AE23" s="1"/>
@@ -1469,7 +1476,7 @@
       <c r="AC24" s="19">
         <v>10</v>
       </c>
-      <c r="AD24" s="33" t="s">
+      <c r="AD24" s="30" t="s">
         <v>39</v>
       </c>
       <c r="AE24" s="1"/>
@@ -1550,6 +1557,10 @@
       <c r="T29" s="1"/>
       <c r="X29" s="1"/>
       <c r="AB29" s="1"/>
+      <c r="AC29" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD29" s="36"/>
       <c r="AE29" s="1"/>
       <c r="AI29" s="1"/>
       <c r="AM29" s="1"/>
@@ -1562,6 +1573,10 @@
       <c r="T30" s="1"/>
       <c r="X30" s="1"/>
       <c r="AB30" s="1"/>
+      <c r="AC30" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD30" s="19"/>
       <c r="AE30" s="1"/>
       <c r="AI30" s="1"/>
       <c r="AM30" s="1"/>
@@ -1574,6 +1589,12 @@
       <c r="T31" s="1"/>
       <c r="X31" s="1"/>
       <c r="AB31" s="1"/>
+      <c r="AC31" s="39">
+        <v>1</v>
+      </c>
+      <c r="AD31" s="29" t="s">
+        <v>36</v>
+      </c>
       <c r="AE31" s="1"/>
       <c r="AI31" s="1"/>
       <c r="AM31" s="1"/>
@@ -1586,6 +1607,12 @@
       <c r="T32" s="1"/>
       <c r="X32" s="1"/>
       <c r="AB32" s="1"/>
+      <c r="AC32" s="39">
+        <v>2</v>
+      </c>
+      <c r="AD32" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="AE32" s="1"/>
       <c r="AI32" s="1"/>
       <c r="AM32" s="1"/>
@@ -1598,6 +1625,12 @@
       <c r="T33" s="1"/>
       <c r="X33" s="1"/>
       <c r="AB33" s="1"/>
+      <c r="AC33" s="39">
+        <v>3</v>
+      </c>
+      <c r="AD33" s="16" t="s">
+        <v>27</v>
+      </c>
       <c r="AE33" s="1"/>
       <c r="AI33" s="1"/>
       <c r="AM33" s="1"/>
@@ -1610,6 +1643,12 @@
       <c r="T34" s="1"/>
       <c r="X34" s="1"/>
       <c r="AB34" s="1"/>
+      <c r="AC34" s="39">
+        <v>4</v>
+      </c>
+      <c r="AD34" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="AE34" s="1"/>
       <c r="AI34" s="1"/>
       <c r="AM34" s="1"/>
@@ -1622,6 +1661,12 @@
       <c r="T35" s="1"/>
       <c r="X35" s="1"/>
       <c r="AB35" s="1"/>
+      <c r="AC35" s="39">
+        <v>5</v>
+      </c>
+      <c r="AD35" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="AE35" s="1"/>
       <c r="AI35" s="1"/>
       <c r="AM35" s="1"/>
@@ -1634,6 +1679,12 @@
       <c r="T36" s="1"/>
       <c r="X36" s="1"/>
       <c r="AB36" s="1"/>
+      <c r="AC36" s="39">
+        <v>6</v>
+      </c>
+      <c r="AD36" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="AE36" s="1"/>
       <c r="AI36" s="1"/>
       <c r="AM36" s="1"/>
@@ -13195,12 +13246,13 @@
       <c r="AM999" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AJ1:AL1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AC29:AD29"/>
     <mergeCell ref="AC14:AD14"/>
     <mergeCell ref="AC21:AD21"/>
     <mergeCell ref="AC1:AD1"/>

</xml_diff>

<commit_message>
teste sd + rfid ruins
</commit_message>
<xml_diff>
--- a/Docs/PINAGEM.xlsx
+++ b/Docs/PINAGEM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconr\Documents\GitHub\choppbot\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconr\Documents\GitHub\MarSidFla\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3E4AD4-68A5-4370-95DA-0D67793DB52A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC5D5A7-DAF3-4797-9B1A-9128ACBA94C7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,15 +461,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -477,6 +468,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -796,7 +796,7 @@
   <dimension ref="A1:AM999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -830,69 +830,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="25"/>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
       <c r="L1" s="25"/>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
       <c r="P1" s="25"/>
-      <c r="Q1" s="38" t="s">
+      <c r="Q1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
       <c r="T1" s="25"/>
-      <c r="U1" s="38" t="s">
+      <c r="U1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
       <c r="X1" s="25"/>
-      <c r="Y1" s="38" t="s">
+      <c r="Y1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
       <c r="AB1" s="26"/>
-      <c r="AC1" s="37" t="s">
+      <c r="AC1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="AD1" s="37"/>
+      <c r="AD1" s="41"/>
       <c r="AE1" s="28"/>
-      <c r="AF1" s="38" t="s">
+      <c r="AF1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="38"/>
+      <c r="AG1" s="39"/>
+      <c r="AH1" s="39"/>
       <c r="AI1" s="25"/>
-      <c r="AJ1" s="38" t="s">
+      <c r="AJ1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="AK1" s="38"/>
-      <c r="AL1" s="38"/>
+      <c r="AK1" s="39"/>
+      <c r="AL1" s="39"/>
       <c r="AM1" s="25"/>
     </row>
     <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41">
-        <v>11</v>
+      <c r="A2" s="38">
+        <v>24</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>12</v>
@@ -961,10 +961,10 @@
         <v>25</v>
       </c>
       <c r="AB2" s="11"/>
-      <c r="AC2" s="36" t="s">
+      <c r="AC2" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="AD2" s="36"/>
+      <c r="AD2" s="40"/>
       <c r="AE2" s="11"/>
       <c r="AF2" s="22">
         <v>45</v>
@@ -982,7 +982,7 @@
       <c r="AK2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="AL2" s="40" t="s">
+      <c r="AL2" s="37" t="s">
         <v>45</v>
       </c>
       <c r="AM2" s="11"/>
@@ -1022,7 +1022,7 @@
         <v>21</v>
       </c>
       <c r="AB3" s="11"/>
-      <c r="AC3" s="39">
+      <c r="AC3" s="36">
         <v>20</v>
       </c>
       <c r="AD3" s="17" t="s">
@@ -1076,7 +1076,7 @@
         <v>23</v>
       </c>
       <c r="AB4" s="11"/>
-      <c r="AC4" s="39">
+      <c r="AC4" s="36">
         <v>21</v>
       </c>
       <c r="AD4" s="16" t="s">
@@ -1154,10 +1154,10 @@
         <v>18</v>
       </c>
       <c r="AB6" s="11"/>
-      <c r="AC6" s="36" t="s">
+      <c r="AC6" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="AD6" s="36"/>
+      <c r="AD6" s="40"/>
       <c r="AE6" s="11"/>
       <c r="AI6" s="11"/>
       <c r="AM6" s="11"/>
@@ -1301,10 +1301,10 @@
       <c r="T14" s="1"/>
       <c r="X14" s="1"/>
       <c r="AB14" s="1"/>
-      <c r="AC14" s="36" t="s">
+      <c r="AC14" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="AD14" s="36"/>
+      <c r="AD14" s="40"/>
       <c r="AE14" s="1"/>
       <c r="AI14" s="1"/>
       <c r="AM14" s="1"/>
@@ -1421,10 +1421,10 @@
       <c r="T21" s="1"/>
       <c r="X21" s="1"/>
       <c r="AB21" s="1"/>
-      <c r="AC21" s="36" t="s">
+      <c r="AC21" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="AD21" s="36"/>
+      <c r="AD21" s="40"/>
       <c r="AE21" s="1"/>
       <c r="AI21" s="1"/>
       <c r="AM21" s="1"/>
@@ -1557,10 +1557,10 @@
       <c r="T29" s="1"/>
       <c r="X29" s="1"/>
       <c r="AB29" s="1"/>
-      <c r="AC29" s="36" t="s">
+      <c r="AC29" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="AD29" s="36"/>
+      <c r="AD29" s="40"/>
       <c r="AE29" s="1"/>
       <c r="AI29" s="1"/>
       <c r="AM29" s="1"/>
@@ -1589,7 +1589,7 @@
       <c r="T31" s="1"/>
       <c r="X31" s="1"/>
       <c r="AB31" s="1"/>
-      <c r="AC31" s="39">
+      <c r="AC31" s="36">
         <v>1</v>
       </c>
       <c r="AD31" s="29" t="s">
@@ -1607,7 +1607,7 @@
       <c r="T32" s="1"/>
       <c r="X32" s="1"/>
       <c r="AB32" s="1"/>
-      <c r="AC32" s="39">
+      <c r="AC32" s="36">
         <v>2</v>
       </c>
       <c r="AD32" s="17" t="s">
@@ -1625,7 +1625,7 @@
       <c r="T33" s="1"/>
       <c r="X33" s="1"/>
       <c r="AB33" s="1"/>
-      <c r="AC33" s="39">
+      <c r="AC33" s="36">
         <v>3</v>
       </c>
       <c r="AD33" s="16" t="s">
@@ -1643,7 +1643,7 @@
       <c r="T34" s="1"/>
       <c r="X34" s="1"/>
       <c r="AB34" s="1"/>
-      <c r="AC34" s="39">
+      <c r="AC34" s="36">
         <v>4</v>
       </c>
       <c r="AD34" s="19" t="s">
@@ -1661,7 +1661,7 @@
       <c r="T35" s="1"/>
       <c r="X35" s="1"/>
       <c r="AB35" s="1"/>
-      <c r="AC35" s="39">
+      <c r="AC35" s="36">
         <v>5</v>
       </c>
       <c r="AD35" s="32" t="s">
@@ -1679,7 +1679,7 @@
       <c r="T36" s="1"/>
       <c r="X36" s="1"/>
       <c r="AB36" s="1"/>
-      <c r="AC36" s="39">
+      <c r="AC36" s="36">
         <v>6</v>
       </c>
       <c r="AD36" s="10" t="s">
@@ -13247,11 +13247,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="AJ1:AL1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AC6:AD6"/>
     <mergeCell ref="AC29:AD29"/>
     <mergeCell ref="AC14:AD14"/>
     <mergeCell ref="AC21:AD21"/>
@@ -13262,6 +13257,11 @@
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="U1:W1"/>
     <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="AJ1:AL1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AC6:AD6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Uma PORRADA de coisas
RFID funcionando, SD funcionando, Inicio do Banco de dados, ja com arquivos reais, Led de RFID, Buzzer, Ajustes gerais
</commit_message>
<xml_diff>
--- a/Docs/PINAGEM.xlsx
+++ b/Docs/PINAGEM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconr\Documents\GitHub\MarSidFla\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITREP\ChoppBot\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707E45A1-17DD-4366-86F4-3EADA7F1BB12}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{15A423EE-5436-410E-B3ED-C5AF3C1601BC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>SD</t>
   </si>
@@ -158,6 +158,39 @@
   </si>
   <si>
     <t>lado botao</t>
+  </si>
+  <si>
+    <t>RFID MURCH</t>
+  </si>
+  <si>
+    <t>sck</t>
+  </si>
+  <si>
+    <t>miso</t>
+  </si>
+  <si>
+    <t>cs</t>
+  </si>
+  <si>
+    <t>pula</t>
+  </si>
+  <si>
+    <t>mosi</t>
+  </si>
+  <si>
+    <t>5v</t>
+  </si>
+  <si>
+    <t>LED RFID</t>
+  </si>
+  <si>
+    <t>ctPINO_LED_RFID</t>
+  </si>
+  <si>
+    <t>ctPINO_BUZZER</t>
+  </si>
+  <si>
+    <t>BUZZER</t>
   </si>
 </sst>
 </file>
@@ -455,13 +488,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -778,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM999"/>
+  <dimension ref="A1:AV999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+      <selection activeCell="AT2" sqref="AT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -812,70 +845,94 @@
     <col min="36" max="37" width="3" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="8.85546875" customWidth="1"/>
     <col min="39" max="39" width="3.85546875" customWidth="1"/>
+    <col min="40" max="40" width="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="3.7109375" customWidth="1"/>
+    <col min="43" max="43" width="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:48" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="25"/>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
       <c r="L1" s="25"/>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
       <c r="P1" s="25"/>
-      <c r="Q1" s="40" t="s">
+      <c r="Q1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
       <c r="T1" s="25"/>
-      <c r="U1" s="40" t="s">
+      <c r="U1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
       <c r="X1" s="25"/>
-      <c r="Y1" s="40" t="s">
+      <c r="Y1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
       <c r="AB1" s="26"/>
-      <c r="AC1" s="39" t="s">
+      <c r="AC1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="AD1" s="39"/>
+      <c r="AD1" s="40"/>
       <c r="AE1" s="28"/>
-      <c r="AF1" s="40" t="s">
+      <c r="AF1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="40"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
       <c r="AI1" s="25"/>
-      <c r="AJ1" s="40" t="s">
+      <c r="AJ1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="AK1" s="40"/>
-      <c r="AL1" s="40"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
       <c r="AM1" s="25"/>
-    </row>
-    <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN1" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
+      <c r="AQ1" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR1" s="38"/>
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU1" s="38"/>
+      <c r="AV1" s="38"/>
+    </row>
+    <row r="2" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <v>24</v>
       </c>
@@ -946,10 +1003,10 @@
         <v>24</v>
       </c>
       <c r="AB2" s="11"/>
-      <c r="AC2" s="38" t="s">
+      <c r="AC2" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="AD2" s="38"/>
+      <c r="AD2" s="39"/>
       <c r="AE2" s="11"/>
       <c r="AF2" s="22">
         <v>45</v>
@@ -971,8 +1028,29 @@
         <v>43</v>
       </c>
       <c r="AM2" s="11"/>
-    </row>
-    <row r="3" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN2" s="2">
+        <v>52</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP2" s="6"/>
+      <c r="AQ2" s="2">
+        <v>26</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS2" s="17"/>
+      <c r="AT2" s="2">
+        <v>32</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AV2" s="17"/>
+    </row>
+    <row r="3" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>51</v>
       </c>
@@ -1034,8 +1112,17 @@
         <v>23</v>
       </c>
       <c r="AM3" s="11"/>
-    </row>
-    <row r="4" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN3" s="2">
+        <v>50</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP3" s="10"/>
+      <c r="AS3" s="16"/>
+      <c r="AV3" s="16"/>
+    </row>
+    <row r="4" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>50</v>
       </c>
@@ -1088,8 +1175,17 @@
         <v>26</v>
       </c>
       <c r="AM4" s="11"/>
-    </row>
-    <row r="5" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN4" s="2">
+        <v>51</v>
+      </c>
+      <c r="AO4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP4" s="16"/>
+      <c r="AS4" s="10"/>
+      <c r="AV4" s="10"/>
+    </row>
+    <row r="5" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>52</v>
       </c>
@@ -1118,8 +1214,17 @@
       <c r="AE5" s="11"/>
       <c r="AI5" s="11"/>
       <c r="AM5" s="11"/>
-    </row>
-    <row r="6" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN5" s="2">
+        <v>53</v>
+      </c>
+      <c r="AO5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP5" s="17"/>
+      <c r="AS5" s="16"/>
+      <c r="AV5" s="16"/>
+    </row>
+    <row r="6" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="11"/>
@@ -1139,15 +1244,22 @@
         <v>18</v>
       </c>
       <c r="AB6" s="11"/>
-      <c r="AC6" s="38" t="s">
+      <c r="AC6" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="AD6" s="38"/>
+      <c r="AD6" s="39"/>
       <c r="AE6" s="11"/>
       <c r="AI6" s="11"/>
       <c r="AM6" s="11"/>
-    </row>
-    <row r="7" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AO6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR6" s="14"/>
+      <c r="AS6" s="17"/>
+      <c r="AU6" s="14"/>
+      <c r="AV6" s="17"/>
+    </row>
+    <row r="7" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15"/>
       <c r="D7" s="11"/>
       <c r="H7" s="11"/>
@@ -1166,8 +1278,13 @@
       <c r="AE7" s="11"/>
       <c r="AI7" s="11"/>
       <c r="AM7" s="11"/>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN7"/>
+      <c r="AO7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP7"/>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B8" s="33"/>
       <c r="D8" s="1"/>
       <c r="H8" s="11"/>
@@ -1185,8 +1302,13 @@
       <c r="AE8" s="1"/>
       <c r="AI8" s="1"/>
       <c r="AM8" s="1"/>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO8" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR8" s="2"/>
+      <c r="AU8" s="2"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
       <c r="H9" s="11"/>
       <c r="L9" s="11"/>
@@ -1204,8 +1326,14 @@
       <c r="AE9" s="1"/>
       <c r="AI9" s="1"/>
       <c r="AM9" s="1"/>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR9" s="15"/>
+      <c r="AU9" s="15"/>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
       <c r="H10" s="11"/>
       <c r="L10" s="11"/>
@@ -1224,8 +1352,12 @@
       <c r="AE10" s="1"/>
       <c r="AI10" s="1"/>
       <c r="AM10" s="1"/>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="15"/>
+      <c r="AT10" s="3"/>
+      <c r="AU10" s="15"/>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
       <c r="H11" s="11"/>
       <c r="L11" s="11"/>
@@ -1243,8 +1375,11 @@
       <c r="AE11" s="1"/>
       <c r="AI11" s="1"/>
       <c r="AM11" s="1"/>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN11" s="3"/>
+      <c r="AQ11" s="3"/>
+      <c r="AT11" s="3"/>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="H12" s="11"/>
       <c r="L12" s="11"/>
@@ -1262,7 +1397,7 @@
       <c r="AI12" s="1"/>
       <c r="AM12" s="1"/>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="H13" s="11"/>
       <c r="L13" s="11"/>
@@ -1274,7 +1409,7 @@
       <c r="AI13" s="1"/>
       <c r="AM13" s="1"/>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="H14" s="11"/>
       <c r="L14" s="11"/>
@@ -1282,15 +1417,15 @@
       <c r="T14" s="1"/>
       <c r="X14" s="1"/>
       <c r="AB14" s="1"/>
-      <c r="AC14" s="38" t="s">
+      <c r="AC14" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="AD14" s="38"/>
+      <c r="AD14" s="39"/>
       <c r="AE14" s="1"/>
       <c r="AI14" s="1"/>
       <c r="AM14" s="1"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="H15" s="11"/>
       <c r="L15" s="11"/>
@@ -1308,7 +1443,7 @@
       <c r="AI15" s="1"/>
       <c r="AM15" s="1"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="H16" s="11"/>
       <c r="L16" s="11"/>
@@ -1402,10 +1537,10 @@
       <c r="T21" s="1"/>
       <c r="X21" s="1"/>
       <c r="AB21" s="1"/>
-      <c r="AC21" s="38" t="s">
+      <c r="AC21" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="AD21" s="38"/>
+      <c r="AD21" s="39"/>
       <c r="AE21" s="1"/>
       <c r="AI21" s="1"/>
       <c r="AM21" s="1"/>
@@ -1538,10 +1673,10 @@
       <c r="T29" s="1"/>
       <c r="X29" s="1"/>
       <c r="AB29" s="1"/>
-      <c r="AC29" s="38" t="s">
+      <c r="AC29" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="AD29" s="38"/>
+      <c r="AD29" s="39"/>
       <c r="AE29" s="1"/>
       <c r="AI29" s="1"/>
       <c r="AM29" s="1"/>
@@ -13227,22 +13362,25 @@
       <c r="AM999" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="AJ1:AL1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AC6:AD6"/>
+  <mergeCells count="18">
+    <mergeCell ref="AT1:AV1"/>
     <mergeCell ref="AC29:AD29"/>
     <mergeCell ref="AC14:AD14"/>
     <mergeCell ref="AC21:AD21"/>
     <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="U1:W1"/>
+    <mergeCell ref="AQ1:AS1"/>
     <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="AJ1:AL1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="AN1:AP1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>